<commit_message>
Removed apache-poi library from dir
</commit_message>
<xml_diff>
--- a/data1.xlsx
+++ b/data1.xlsx
@@ -30,9 +30,6 @@
     <t>Phone</t>
   </si>
   <si>
-    <t>ParentEmail</t>
-  </si>
-  <si>
     <t>Subject</t>
   </si>
   <si>
@@ -42,9 +39,6 @@
     <t>Availability</t>
   </si>
   <si>
-    <t>RequestVolunteer</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -184,6 +178,12 @@
   </si>
   <si>
     <t>Requested Student</t>
+  </si>
+  <si>
+    <t>Parent Email</t>
+  </si>
+  <si>
+    <t>Requested Volunteer</t>
   </si>
 </sst>
 </file>
@@ -526,7 +526,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,10 +536,10 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -554,165 +554,165 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" t="s">
         <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C2">
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F2">
         <v>7324591010</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C3">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F3">
         <v>6098471068</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" t="s">
         <v>14</v>
       </c>
-      <c r="I3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" t="s">
-        <v>16</v>
-      </c>
       <c r="L3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" t="s">
         <v>27</v>
       </c>
-      <c r="F4" t="s">
-        <v>53</v>
-      </c>
-      <c r="G4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" t="s">
         <v>24</v>
-      </c>
-      <c r="J4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" t="s">
         <v>45</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
         <v>46</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" t="s">
         <v>47</v>
       </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" t="s">
         <v>48</v>
       </c>
-      <c r="F5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="J5" t="s">
         <v>49</v>
       </c>
-      <c r="H5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>50</v>
       </c>
-      <c r="J5" t="s">
-        <v>51</v>
-      </c>
-      <c r="K5" t="s">
-        <v>52</v>
-      </c>
       <c r="L5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -725,7 +725,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,10 +735,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -750,42 +750,42 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" t="s">
         <v>32</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>33</v>
       </c>
-      <c r="H1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J1" t="s">
-        <v>35</v>
-      </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C2">
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G2">
         <v>7326059815</v>

</xml_diff>

<commit_message>
Manual Pair and Letter Generation
</commit_message>
<xml_diff>
--- a/data1.xlsx
+++ b/data1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="3" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="93">
   <si>
     <t>Grade</t>
   </si>
@@ -57,12 +57,6 @@
     <t>Both</t>
   </si>
   <si>
-    <t>MTWThF</t>
-  </si>
-  <si>
-    <t>4 Muirfield Blvd</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -84,15 +78,6 @@
     <t>Special Needs Preference</t>
   </si>
   <si>
-    <t>Roland</t>
-  </si>
-  <si>
-    <t>Fong</t>
-  </si>
-  <si>
-    <t>rfblue2@gmail.com</t>
-  </si>
-  <si>
     <t>Mary</t>
   </si>
   <si>
@@ -147,9 +132,6 @@
     <t>Summer</t>
   </si>
   <si>
-    <t>TTh</t>
-  </si>
-  <si>
     <t>3 Hollywood Dr.</t>
   </si>
   <si>
@@ -189,9 +171,6 @@
     <t>234567</t>
   </si>
   <si>
-    <t>WThF</t>
-  </si>
-  <si>
     <t>9 Melody Dr.</t>
   </si>
   <si>
@@ -228,43 +207,94 @@
     <t>Student</t>
   </si>
   <si>
-    <t>TThF</t>
-  </si>
-  <si>
     <t>A Disney Character</t>
   </si>
   <si>
-    <t>Bob</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>Lala</t>
   </si>
   <si>
     <t>Haha</t>
   </si>
   <si>
-    <t>K</t>
-  </si>
-  <si>
     <t>0 Fantasy Ln</t>
   </si>
   <si>
-    <t>6665554444</t>
-  </si>
-  <si>
-    <t>dodo@yoyo.com</t>
-  </si>
-  <si>
-    <t>Fall</t>
-  </si>
-  <si>
-    <t>MTThF</t>
-  </si>
-  <si>
-    <t>Weird</t>
+    <t>BCEFHIKL</t>
+  </si>
+  <si>
+    <t>CFIL</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Hank Lewis</t>
+  </si>
+  <si>
+    <t>Minnie Mouse</t>
+  </si>
+  <si>
+    <t>BCEFHIKJNOQ</t>
+  </si>
+  <si>
+    <t>Anna</t>
+  </si>
+  <si>
+    <t>Arendelle</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>1 Castle Place</t>
+  </si>
+  <si>
+    <t>8374829993</t>
+  </si>
+  <si>
+    <t>aorg@gmail.com</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>BCDEF</t>
+  </si>
+  <si>
+    <t>Kristoff</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>9 Ice St</t>
+  </si>
+  <si>
+    <t>kristoff@yahoo.com</t>
+  </si>
+  <si>
+    <t>Anna Arendelle</t>
+  </si>
+  <si>
+    <t>45678</t>
+  </si>
+  <si>
+    <t>Kristoff O</t>
+  </si>
+  <si>
+    <t>Lala Haha</t>
+  </si>
+  <si>
+    <t>Requested Subject</t>
+  </si>
+  <si>
+    <t>Michelle Kappa</t>
+  </si>
+  <si>
+    <t>lala@lala.com</t>
+  </si>
+  <si>
+    <t>EFHIKL</t>
   </si>
 </sst>
 </file>
@@ -305,8 +335,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,13 +652,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1" s="2">
-        <v>41794</v>
-      </c>
-      <c r="C1" s="2">
-        <v>41881</v>
+        <v>60</v>
+      </c>
+      <c r="B1" s="1">
+        <v>41911</v>
+      </c>
+      <c r="C1" s="1">
+        <v>41985</v>
       </c>
     </row>
   </sheetData>
@@ -639,10 +669,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,13 +682,13 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -673,7 +703,7 @@
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -685,13 +715,13 @@
         <v>6</v>
       </c>
       <c r="L1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="M1" t="s">
         <v>7</v>
       </c>
       <c r="N1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -699,43 +729,43 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="G2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="I2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="J2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="K2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" t="s">
+        <v>63</v>
+      </c>
+      <c r="N2" t="s">
         <v>70</v>
-      </c>
-      <c r="L2" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" t="s">
-        <v>71</v>
-      </c>
-      <c r="N2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -743,25 +773,25 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="G3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="H3" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="I3" t="s">
         <v>9</v>
@@ -770,39 +800,42 @@
         <v>10</v>
       </c>
       <c r="K3" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="L3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="M3" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="N3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="H4" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="I4" t="s">
         <v>12</v>
@@ -811,57 +844,60 @@
         <v>10</v>
       </c>
       <c r="K4" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="L4" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="M4" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="N4" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>73</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>74</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>75</v>
-      </c>
-      <c r="D5" t="s">
-        <v>76</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
       </c>
       <c r="F5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G5" t="s">
         <v>77</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>78</v>
-      </c>
-      <c r="H5" t="s">
-        <v>79</v>
       </c>
       <c r="I5" t="s">
         <v>12</v>
       </c>
       <c r="J5" t="s">
+        <v>79</v>
+      </c>
+      <c r="K5" t="s">
         <v>80</v>
       </c>
-      <c r="K5" t="s">
-        <v>81</v>
-      </c>
       <c r="L5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="M5" t="s">
-        <v>82</v>
+        <v>13</v>
       </c>
       <c r="N5" t="s">
-        <v>15</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -871,26 +907,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -902,133 +939,172 @@
         <v>2</v>
       </c>
       <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>19</v>
       </c>
-      <c r="I1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" t="s">
-        <v>69</v>
+      <c r="O1" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2">
-        <v>12</v>
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="G2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2">
-        <v>7326059815</v>
-      </c>
-      <c r="J2" s="1">
-        <v>678</v>
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" t="s">
+        <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
         <v>45</v>
       </c>
       <c r="G3" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="J3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="K3" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="L3" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="M3" t="s">
+        <v>69</v>
+      </c>
+      <c r="N3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>47</v>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="G4" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="H4" t="s">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="I4" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="J4" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="K4" t="s">
-        <v>15</v>
+        <v>86</v>
       </c>
       <c r="L4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="M4" t="s">
-        <v>61</v>
+        <v>69</v>
+      </c>
+      <c r="N4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
File Chooser for letters
</commit_message>
<xml_diff>
--- a/data1.xlsx
+++ b/data1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="107">
   <si>
     <t>Grade</t>
   </si>
@@ -295,6 +295,48 @@
   </si>
   <si>
     <t>EFHIKL</t>
+  </si>
+  <si>
+    <t>Bjorgman</t>
+  </si>
+  <si>
+    <t>Elsa</t>
+  </si>
+  <si>
+    <t>Kristoff Bjorgman</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Hans</t>
+  </si>
+  <si>
+    <t>Westerguard</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>9 Southern Isles</t>
+  </si>
+  <si>
+    <t>hans_westerguard@gmail.com</t>
+  </si>
+  <si>
+    <t>9882227462</t>
+  </si>
+  <si>
+    <t>EFHIKQ</t>
+  </si>
+  <si>
+    <t>Evil</t>
+  </si>
+  <si>
+    <t>Hans Westerguard</t>
+  </si>
+  <si>
+    <t>Elsa Arendelle</t>
   </si>
 </sst>
 </file>
@@ -779,7 +821,7 @@
         <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>96</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -897,7 +939,51 @@
         <v>13</v>
       </c>
       <c r="N5" t="s">
-        <v>87</v>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H6" t="s">
+        <v>78</v>
+      </c>
+      <c r="I6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" t="s">
+        <v>79</v>
+      </c>
+      <c r="K6" t="s">
+        <v>80</v>
+      </c>
+      <c r="L6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6" t="s">
+        <v>13</v>
+      </c>
+      <c r="N6" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1068,7 +1154,7 @@
         <v>81</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="D4" t="s">
         <v>27</v>
@@ -1105,6 +1191,53 @@
       </c>
       <c r="O4" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G5" t="s">
+        <v>101</v>
+      </c>
+      <c r="H5" t="s">
+        <v>102</v>
+      </c>
+      <c r="I5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" t="s">
+        <v>85</v>
+      </c>
+      <c r="K5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" t="s">
+        <v>103</v>
+      </c>
+      <c r="N5" t="s">
+        <v>104</v>
+      </c>
+      <c r="O5" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>